<commit_message>
Adicionando mais funções e fazendo o boletim
</commit_message>
<xml_diff>
--- a/Casos-de-Teste.xlsx
+++ b/Casos-de-Teste.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29203"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola_teste-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola_testepy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1C5537-AA8F-452D-B099-B454E88DF2A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA62E2DF-D0D6-40F5-BBAB-35E0479613F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{06FDE838-307B-407B-A4F2-DD8BF9EE4C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>ARQUIVO</t>
   </si>
@@ -36,12 +47,12 @@
     <t>DESCRIÇÃO</t>
   </si>
   <si>
+    <t>ENTRADA</t>
+  </si>
+  <si>
     <t>SAÍDA</t>
   </si>
   <si>
-    <t>ENTRADA</t>
-  </si>
-  <si>
     <t>escola/aluno.py</t>
   </si>
   <si>
@@ -51,18 +62,27 @@
     <t>Calculo Básico</t>
   </si>
   <si>
+    <t>[10.0, 5.0, 6.0, 1.0]</t>
+  </si>
+  <si>
     <t>5.5</t>
   </si>
   <si>
     <t>Calculo Básico com notas apenas 0</t>
   </si>
   <si>
+    <t>[0.0, 0.0, 0.0, 0.0]</t>
+  </si>
+  <si>
     <t>0.0</t>
   </si>
   <si>
     <t>Calculo Básico com notas apenas 10</t>
   </si>
   <si>
+    <t>[10.0, 10.0, 10.0, 10.0]</t>
+  </si>
+  <si>
     <t>10.0</t>
   </si>
   <si>
@@ -75,50 +95,92 @@
     <t>7.0</t>
   </si>
   <si>
-    <t>Calculo Básico com 7 notas</t>
-  </si>
-  <si>
-    <t>[5.0, 8,8, 6.7, 2.0, 5.3, 8.8, 9.9]</t>
-  </si>
-  <si>
-    <t>[10.0, 10.0, 10.0, 10.0]</t>
-  </si>
-  <si>
-    <t>[0.0, 0.0, 0.0, 0.0]</t>
-  </si>
-  <si>
-    <t>[10.0, 5.0, 6.0, 1.0]</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>Testando o arredondamento</t>
-  </si>
-  <si>
-    <t>[5.8, 9.3]</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>7.6</t>
-  </si>
-  <si>
-    <t>7.7</t>
-  </si>
-  <si>
-    <t>Testando o arredondamento decimal maior que 0.56</t>
-  </si>
-  <si>
-    <t>Testando o arredondamento decimal de 0.55</t>
+    <t>Calculo Básico com lista vazia</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>ValueError("Não é permitido uma lista vazia")</t>
+  </si>
+  <si>
+    <t>Testando uma string ao inves de uma lista</t>
+  </si>
+  <si>
+    <t>["ola"]</t>
+  </si>
+  <si>
+    <t>TypeError("nota inválida")</t>
+  </si>
+  <si>
+    <t>Enviando uma string como nota</t>
+  </si>
+  <si>
+    <t>["ola",3.0]</t>
+  </si>
+  <si>
+    <t>Enviando uma nota negativa</t>
+  </si>
+  <si>
+    <t>[-5.8]</t>
+  </si>
+  <si>
+    <t>ValueError("Limite atingido")</t>
+  </si>
+  <si>
+    <t>PARMERA</t>
+  </si>
+  <si>
+    <t>escola/boletim.py</t>
+  </si>
+  <si>
+    <t>calcular_media_boletim</t>
+  </si>
+  <si>
+    <t>Se a soma das notas for menor que 7 e maior que 5</t>
+  </si>
+  <si>
+    <t>recuperação</t>
+  </si>
+  <si>
+    <t>Se a soma das notas for maior ou igual a 7</t>
+  </si>
+  <si>
+    <t>[10.0, 5.0, 7.0, 7.0]</t>
+  </si>
+  <si>
+    <t>aprovado</t>
+  </si>
+  <si>
+    <t>Se a soma das notas for menor ou igual a 4.9</t>
+  </si>
+  <si>
+    <t>[2.0, 5.0, 7.0, 3.0]</t>
+  </si>
+  <si>
+    <t>reprovado</t>
+  </si>
+  <si>
+    <t>calculo com menos de 4 notas</t>
+  </si>
+  <si>
+    <t>[4.0,7.0,9.0]</t>
+  </si>
+  <si>
+    <t>ValueError("notas insuficientes ")</t>
+  </si>
+  <si>
+    <t>Enviando uma nota maior que 10</t>
+  </si>
+  <si>
+    <t>[9,11,10]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,16 +188,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,17 +223,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -170,7 +274,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -466,22 +570,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FCC92D-FF06-445D-A5CC-E477BF905430}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,13 +596,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -509,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -523,16 +627,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -540,16 +644,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -557,16 +661,16 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -574,16 +678,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -600,7 +704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -608,16 +712,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -628,13 +732,178 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fiz as validações de acordo com a planilha do excel, 100% de exito
</commit_message>
<xml_diff>
--- a/Casos-de-Teste.xlsx
+++ b/Casos-de-Teste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20343"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola_teste-python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola_testepy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1C5537-AA8F-452D-B099-B454E88DF2A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A2E0AE-C0B7-42C6-B828-2560C8BAC1EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{06FDE838-307B-407B-A4F2-DD8BF9EE4C94}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>ARQUIVO</t>
   </si>
@@ -75,12 +75,6 @@
     <t>7.0</t>
   </si>
   <si>
-    <t>Calculo Básico com 7 notas</t>
-  </si>
-  <si>
-    <t>[5.0, 8,8, 6.7, 2.0, 5.3, 8.8, 9.9]</t>
-  </si>
-  <si>
     <t>[10.0, 10.0, 10.0, 10.0]</t>
   </si>
   <si>
@@ -90,35 +84,92 @@
     <t>[10.0, 5.0, 6.0, 1.0]</t>
   </si>
   <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>Testando o arredondamento</t>
-  </si>
-  <si>
-    <t>[5.8, 9.3]</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>7.6</t>
-  </si>
-  <si>
-    <t>7.7</t>
-  </si>
-  <si>
-    <t>Testando o arredondamento decimal maior que 0.56</t>
-  </si>
-  <si>
-    <t>Testando o arredondamento decimal de 0.55</t>
+    <t>ValueError("Não é permitido uma lista vazia")</t>
+  </si>
+  <si>
+    <t>TypeError("nota inválida")</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Calculo Básico com lista vazia</t>
+  </si>
+  <si>
+    <t>Testando uma string ao inves de uma lista</t>
+  </si>
+  <si>
+    <t>["ola"]</t>
+  </si>
+  <si>
+    <t>["ola",3.0]</t>
+  </si>
+  <si>
+    <t>Enviando uma nota negativa</t>
+  </si>
+  <si>
+    <t>[-5.8]</t>
+  </si>
+  <si>
+    <t>Enviando uma string como nota</t>
+  </si>
+  <si>
+    <t>ValueError("Limite atingido")</t>
+  </si>
+  <si>
+    <t>PARMERA</t>
+  </si>
+  <si>
+    <t>escola/boletim.py</t>
+  </si>
+  <si>
+    <t>Se a soma das notas for maior ou igual a 7</t>
+  </si>
+  <si>
+    <t>[10.0, 5.0, 7.0, 7.0]</t>
+  </si>
+  <si>
+    <t>[2.0, 5.0, 7.0, 3.0]</t>
+  </si>
+  <si>
+    <t>calcular_media_boletim</t>
+  </si>
+  <si>
+    <t>Se a soma das notas for menor que 7 e maior que 5</t>
+  </si>
+  <si>
+    <t>Se a soma das notas for menor ou igual a 4.9</t>
+  </si>
+  <si>
+    <t>calculo com menos de 4 notas</t>
+  </si>
+  <si>
+    <t>[4.0,7.0,9.0]</t>
+  </si>
+  <si>
+    <t>recuperação</t>
+  </si>
+  <si>
+    <t>aprovado</t>
+  </si>
+  <si>
+    <t>reprovado</t>
+  </si>
+  <si>
+    <t>ValueError("notas insuficientes ")</t>
+  </si>
+  <si>
+    <t>Enviando uma nota maior que 10</t>
+  </si>
+  <si>
+    <t>[9,11,10]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,16 +177,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,17 +212,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Entrada" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,19 +559,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FCC92D-FF06-445D-A5CC-E477BF905430}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -526,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -543,7 +636,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -574,13 +667,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -591,13 +684,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,10 +704,10 @@
         <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,16 +718,181 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>